<commit_message>
Finalizando script de cálculo de métricas
</commit_message>
<xml_diff>
--- a/Dependências/allourideas/TaitiWithdeps-allourideas.xlsx
+++ b/Dependências/allourideas/TaitiWithdeps-allourideas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
   <si>
     <t>Project</t>
   </si>
@@ -139,34 +139,34 @@
     <t>[app/controllers/application_controller.rb, app/controllers/choices_controller.rb, app/controllers/earls_controller.rb, app/controllers/prompts_controller.rb, app/controllers/questions_controller.rb, app/models/earl.rb, app/models/question.rb, app/views/earls/_vote_box_js.html.erb, app/views/questions/new.html.haml, config/routes.rb, features/admin/flag_as_inappropriate_choice.feature, features/admin/toggle_choice_activation.feature, features/idea_marketplaces/create_question.feature, features/step_definitions/admin_steps.rb, features/step_definitions/idea_marketplace_steps.rb, features/support/paths.rb, features/voting/flag_as_inappropriate.feature, public/javascripts/application.js]</t>
   </si>
   <si>
-    <t>['app/controllers/home_controller.rb', ' app/models/question.rb', ' app/views/home/admin.html.haml', ' app/views/shared/_highcharts_header.html.haml']</t>
-  </si>
-  <si>
-    <t>['app/models/choice.rb', ' app/models/earl.rb', ' app/models/item.rb', ' app/models/question.rb', ' app/views/abingo_dashboard/_experiment_row.html.haml', ' app/views/abingo_dashboard/index.html.haml']</t>
-  </si>
-  <si>
-    <t>['app/models/choice.rb', ' app/models/density.rb', ' app/models/earl.rb', ' app/models/prompt.rb', ' app/models/question.rb', ' app/models/session.rb', ' app/views/abingo_dashboard/_experiment_row.html.haml', ' app/views/abingo_dashboard/index.html.haml']</t>
-  </si>
-  <si>
-    <t>['app/views/abingo_dashboard/index.html.haml', 'app/models/question.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml']</t>
-  </si>
-  <si>
-    <t>['app/controllers/choices_controller.rb', ' app/models/choice.rb', ' app/models/earl.rb', ' app/models/prompt.rb', ' app/models/question.rb', ' app/views/abingo_dashboard/_experiment_row.html.haml', ' app/views/abingo_dashboard/index.html.haml', ' app/views/choices/show.html.haml', ' app/views/shared/_header_vote.html.haml']</t>
-  </si>
-  <si>
-    <t>['app/controllers/choices_controller.rb', ' app/controllers/home_controller.rb', ' app/controllers/questions_controller.rb', ' app/models/choice.rb', ' app/models/earl.rb', ' app/models/item.rb', ' app/models/prompt.rb', ' app/models/question.rb', ' app/views/abingo_dashboard/_experiment_row.html.haml', ' app/views/abingo_dashboard/index.html.haml', ' app/views/choices/show.html.haml', ' app/views/home/about.html.haml', ' app/views/home/admin.html.haml', ' app/views/home/index.html.haml', ' app/views/home/privacy.html.haml', ' app/views/questions/_idea.html.haml', ' app/views/questions/about.html.haml', ' app/views/questions/admin.html.haml', ' app/views/questions/new.html.haml', ' app/views/questions/results.html.haml', ' app/views/questions/voter_map.html.erb', ' app/views/questions/word_cloud.html.erb', ' app/views/shared/_google_jsapi.html.haml', ' app/views/shared/_header_vote.html.haml', ' app/views/shared/_highcharts_header.html.haml']</t>
-  </si>
-  <si>
-    <t>['app/models/question.rb', ' app/views/abingo_dashboard/_experiment_row.html.haml', ' app/views/abingo_dashboard/index.html.haml']</t>
-  </si>
-  <si>
-    <t>['app/models/choice.rb', ' app/models/prompt.rb', ' app/models/question.rb', ' app/views/abingo_dashboard/_experiment_row.html.haml', ' app/views/abingo_dashboard/index.html.haml']</t>
-  </si>
-  <si>
-    <t>['app/controllers/choices_controller.rb', ' app/controllers/home_controller.rb', ' app/controllers/questions_controller.rb', ' app/models/choice.rb', ' app/models/earl.rb', ' app/models/item.rb', ' app/models/prompt.rb', ' app/models/question.rb', ' app/models/user.rb', ' app/views/abingo_dashboard/_experiment_row.html.haml', ' app/views/abingo_dashboard/index.html.haml', ' app/views/choices/show.html.haml', ' app/views/home/about.html.haml', ' app/views/home/admin.html.haml', ' app/views/home/index.html.haml', ' app/views/home/privacy.html.haml', ' app/views/questions/_idea.html.haml', ' app/views/questions/about.html.haml', ' app/views/questions/admin.html.haml', ' app/views/questions/new.html.haml', ' app/views/questions/results.html.haml', ' app/views/questions/voter_map.html.erb', ' app/views/questions/word_cloud.html.erb', ' app/views/shared/_google_jsapi.html.haml', ' app/views/shared/_header_vote.html.haml', ' app/views/shared/_highcharts_header.html.haml']</t>
-  </si>
-  <si>
-    <t>['app/models/choice.rb', ' app/models/earl.rb', ' app/models/question.rb', ' app/views/abingo_dashboard/_experiment_row.html.haml', ' app/views/abingo_dashboard/index.html.haml']</t>
+    <t>['app/controllers/home_controller.rb', 'app/models/question.rb', 'app/views/home/admin.html.haml', 'app/views/shared/_highcharts_header.html.haml']</t>
+  </si>
+  <si>
+    <t>['app/models/choice.rb', 'app/models/earl.rb', 'app/models/item.rb', 'app/models/question.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml']</t>
+  </si>
+  <si>
+    <t>['app/models/choice.rb', 'app/models/density.rb', 'app/models/earl.rb', 'app/models/prompt.rb', 'app/models/question.rb', 'app/models/session.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml']</t>
+  </si>
+  <si>
+    <t>['app/views/abingo_dashboard/index.html.haml', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/models/question.rb']</t>
+  </si>
+  <si>
+    <t>['app/controllers/choices_controller.rb', 'app/models/choice.rb', 'app/models/earl.rb', 'app/models/prompt.rb', 'app/models/question.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml', 'app/views/choices/show.html.haml', 'app/views/shared/_header_vote.html.haml']</t>
+  </si>
+  <si>
+    <t>['app/controllers/choices_controller.rb', 'app/controllers/home_controller.rb', 'app/controllers/questions_controller.rb', 'app/models/choice.rb', 'app/models/earl.rb', 'app/models/item.rb', 'app/models/prompt.rb', 'app/models/question.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml', 'app/views/choices/show.html.haml', 'app/views/home/about.html.haml', 'app/views/home/admin.html.haml', 'app/views/home/index.html.haml', 'app/views/home/privacy.html.haml', 'app/views/questions/_idea.html.haml', 'app/views/questions/about.html.haml', 'app/views/questions/admin.html.haml', 'app/views/questions/new.html.haml', 'app/views/questions/results.html.haml', 'app/views/questions/voter_map.html.erb', 'app/views/questions/word_cloud.html.erb', 'app/views/shared/_google_jsapi.html.haml', 'app/views/shared/_header_vote.html.haml', 'app/views/shared/_highcharts_header.html.haml']</t>
+  </si>
+  <si>
+    <t>['app/models/question.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml']</t>
+  </si>
+  <si>
+    <t>['app/models/choice.rb', 'app/models/prompt.rb', 'app/models/question.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml']</t>
+  </si>
+  <si>
+    <t>['app/controllers/choices_controller.rb', 'app/controllers/home_controller.rb', 'app/controllers/questions_controller.rb', 'app/models/choice.rb', 'app/models/earl.rb', 'app/models/item.rb', 'app/models/prompt.rb', 'app/models/question.rb', 'app/models/user.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml', 'app/views/choices/show.html.haml', 'app/views/home/about.html.haml', 'app/views/home/admin.html.haml', 'app/views/home/index.html.haml', 'app/views/home/privacy.html.haml', 'app/views/questions/_idea.html.haml', 'app/views/questions/about.html.haml', 'app/views/questions/admin.html.haml', 'app/views/questions/new.html.haml', 'app/views/questions/results.html.haml', 'app/views/questions/voter_map.html.erb', 'app/views/questions/word_cloud.html.erb', 'app/views/shared/_google_jsapi.html.haml', 'app/views/shared/_header_vote.html.haml', 'app/views/shared/_highcharts_header.html.haml']</t>
+  </si>
+  <si>
+    <t>['app/models/choice.rb', 'app/models/earl.rb', 'app/models/question.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml']</t>
   </si>
   <si>
     <t>Null</t>
@@ -794,22 +794,22 @@
         <v>45</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>51</v>
+        <v>0.0625</v>
+      </c>
+      <c r="I7">
+        <v>0.06849315068493152</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>51</v>
+        <v>0.0625</v>
+      </c>
+      <c r="L7">
+        <v>0.06849315068493152</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -984,22 +984,22 @@
         <v>49</v>
       </c>
       <c r="G12">
-        <v>0.2307692307692308</v>
+        <v>0.2692307692307692</v>
       </c>
       <c r="H12">
-        <v>0.1463414634146341</v>
+        <v>0.1707317073170732</v>
       </c>
       <c r="I12">
-        <v>0.1578947368421053</v>
+        <v>0.1842105263157895</v>
       </c>
       <c r="J12">
-        <v>0.2307692307692308</v>
+        <v>0.2692307692307692</v>
       </c>
       <c r="K12">
-        <v>0.1463414634146341</v>
+        <v>0.1707317073170732</v>
       </c>
       <c r="L12">
-        <v>0.1578947368421053</v>
+        <v>0.1842105263157895</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1022,22 +1022,22 @@
         <v>45</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
-        <v>51</v>
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="I13">
+        <v>0.07692307692307693</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13" t="s">
-        <v>51</v>
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="L13">
+        <v>0.07692307692307693</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1060,22 +1060,22 @@
         <v>50</v>
       </c>
       <c r="G14">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H14">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I14">
-        <v>0.05882352941176471</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="J14">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="K14">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="L14">
-        <v>0.05882352941176471</v>
+        <v>0.1176470588235294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção de pequeno erro
</commit_message>
<xml_diff>
--- a/Dependências/allourideas/TaitiWithdeps-allourideas.xlsx
+++ b/Dependências/allourideas/TaitiWithdeps-allourideas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <t>Project</t>
   </si>
@@ -34,6 +34,9 @@
     <t>TestIWithDeps</t>
   </si>
   <si>
+    <t>IsolatedDeps</t>
+  </si>
+  <si>
     <t>Precision</t>
   </si>
   <si>
@@ -148,7 +151,7 @@
     <t>['app/models/choice.rb', 'app/models/density.rb', 'app/models/earl.rb', 'app/models/prompt.rb', 'app/models/question.rb', 'app/models/session.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml']</t>
   </si>
   <si>
-    <t>['app/views/abingo_dashboard/index.html.haml', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/models/question.rb']</t>
+    <t>['app/views/abingo_dashboard/_experiment_row.html.haml', 'app/models/question.rb', 'app/views/abingo_dashboard/index.html.haml']</t>
   </si>
   <si>
     <t>['app/controllers/choices_controller.rb', 'app/models/choice.rb', 'app/models/earl.rb', 'app/models/prompt.rb', 'app/models/question.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml', 'app/views/choices/show.html.haml', 'app/views/shared/_header_vote.html.haml']</t>
@@ -167,6 +170,12 @@
   </si>
   <si>
     <t>['app/models/choice.rb', 'app/models/earl.rb', 'app/models/question.rb', 'app/views/abingo_dashboard/_experiment_row.html.haml', 'app/views/abingo_dashboard/index.html.haml']</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
   <si>
     <t>Null</t>
@@ -540,13 +549,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,498 +592,540 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2">
         <v>0.25</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.1666666666666667</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.1785714285714285</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.25</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.1666666666666667</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.1785714285714285</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>54</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>54</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>54</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7">
         <v>0.1111111111111111</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.0625</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.06849315068493152</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>0.1111111111111111</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.0625</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.06849315068493152</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>54</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="L9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>54</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>54</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>171</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12">
         <v>0.2692307692307692</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.1707317073170732</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.1842105263157895</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.2692307692307692</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.1707317073170732</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>0.1842105263157895</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>174</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13">
+        <v>46</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13">
         <v>0.1111111111111111</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.07142857142857142</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.07692307692307693</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.1111111111111111</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0.07142857142857142</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.07692307692307693</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>176</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14">
         <v>0.4</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.1</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.1176470588235294</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.4</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.1</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>0.1176470588235294</v>
       </c>
     </row>

</xml_diff>